<commit_message>
Adicionado outra forma de Scroll para agilizar o teste
</commit_message>
<xml_diff>
--- a/target/classes/br/com/rsinet/hub_TDD/DadosTeste/DadosTeste.xlsx
+++ b/target/classes/br/com/rsinet/hub_TDD/DadosTeste/DadosTeste.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{00F02B2B-C94A-401B-80A3-AB5769009589}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{4B6FB65F-3878-49CA-B060-6FDDFB8EE921}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="20880" windowHeight="12930" xr2:uid="{C5C229D6-6427-449A-9BBF-D07F863B75D3}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="20940" windowHeight="12930" xr2:uid="{C5C229D6-6427-449A-9BBF-D07F863B75D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -129,7 +129,7 @@
     <t>usertests356</t>
   </si>
   <si>
-    <t>usertests358</t>
+    <t>usertests360</t>
   </si>
 </sst>
 </file>
@@ -543,7 +543,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Exlusão de alguns arquivos
</commit_message>
<xml_diff>
--- a/target/classes/br/com/rsinet/hub_TDD/DadosTeste/DadosTeste.xlsx
+++ b/target/classes/br/com/rsinet/hub_TDD/DadosTeste/DadosTeste.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{4B6FB65F-3878-49CA-B060-6FDDFB8EE921}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{310047B4-8B1C-49E1-B543-4494BF33B020}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="20940" windowHeight="12930" xr2:uid="{C5C229D6-6427-449A-9BBF-D07F863B75D3}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="20970" windowHeight="11820" xr2:uid="{C5C229D6-6427-449A-9BBF-D07F863B75D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -129,7 +129,7 @@
     <t>usertests356</t>
   </si>
   <si>
-    <t>usertests360</t>
+    <t>usertests361</t>
   </si>
 </sst>
 </file>
@@ -543,7 +543,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>